<commit_message>
update Fig 5 and Table 2 to account for samples with too few UMIs
</commit_message>
<xml_diff>
--- a/SVGs/Table_2.xlsx
+++ b/SVGs/Table_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t xml:space="preserve">RT-LAMP
 Result </t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">35-40</t>
   </si>
   <si>
-    <t xml:space="preserve">undetec*</t>
+    <t xml:space="preserve">too few</t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="28">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -192,11 +192,9 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="thin"/>
+      <right style="double"/>
       <top style="double"/>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -222,7 +220,7 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="thin"/>
+      <right style="double"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
@@ -264,7 +262,7 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right/>
+      <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
@@ -284,17 +282,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top style="double"/>
@@ -317,29 +304,20 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="double"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
+      <right style="double"/>
       <top style="thin"/>
       <bottom style="double"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="double"/>
+      <right style="thin"/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="thin"/>
       <right/>
       <top/>
       <bottom style="thin"/>
@@ -378,7 +356,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -431,111 +409,123 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,7 +554,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -616,10 +606,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AMJ16"/>
+  <dimension ref="B1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -694,60 +684,60 @@
       <c r="E5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="15" t="n">
+      <c r="G5" s="16" t="n">
         <v>49</v>
       </c>
-      <c r="H5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="17" t="n">
+      <c r="H5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="18" t="n">
         <f aca="false">SUM(G5:H5)</f>
         <v>49</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="20" t="n">
+      <c r="G6" s="21" t="n">
         <v>28</v>
       </c>
-      <c r="H6" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22" t="n">
+      <c r="H6" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="23" t="n">
         <f aca="false">SUM(G6:H6)</f>
         <v>28</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="20" t="n">
+      <c r="G7" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="22" t="n">
+      <c r="H7" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="23" t="n">
         <f aca="false">SUM(G7:H7)</f>
         <v>4</v>
       </c>
@@ -760,16 +750,16 @@
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="22" t="n">
+      <c r="G8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="23" t="n">
         <f aca="false">SUM(G8:H8)</f>
         <v>0</v>
       </c>
@@ -783,19 +773,19 @@
         <v>3</v>
       </c>
       <c r="D9" s="13"/>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="28" t="n">
+      <c r="G9" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="29" t="n">
         <f aca="false">SUM(G9:H9)</f>
         <v>0</v>
       </c>
@@ -805,27 +795,27 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="11"/>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="31" t="n">
+      <c r="G10" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="32" t="n">
         <f aca="false">SUM(G10:H10)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -833,19 +823,19 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="11"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="21" t="n">
+      <c r="G11" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="22" t="n">
+      <c r="I11" s="23" t="n">
         <f aca="false">SUM(G11:H11)</f>
         <v>2</v>
       </c>
@@ -855,19 +845,19 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="11"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="21" t="n">
+      <c r="G12" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="I12" s="22" t="n">
+      <c r="I12" s="23" t="n">
         <f aca="false">SUM(G12:H12)</f>
         <v>16</v>
       </c>
@@ -877,19 +867,19 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="24" t="n">
+      <c r="G13" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="25" t="n">
         <v>16</v>
       </c>
-      <c r="I13" s="32" t="n">
+      <c r="I13" s="33" t="n">
         <f aca="false">SUM(G13:H13)</f>
         <v>16</v>
       </c>
@@ -899,81 +889,176 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="11"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="19" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="26" t="n">
+      <c r="G14" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="27" t="n">
-        <v>648</v>
-      </c>
-      <c r="I14" s="28" t="n">
+      <c r="H14" s="28" t="n">
+        <v>637</v>
+      </c>
+      <c r="I14" s="29" t="n">
         <f aca="false">SUM(G14:H14)</f>
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11"/>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="28" t="n">
+      <c r="D15" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="32" t="n">
         <f aca="false">SUM(G15:H15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="37" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="23" t="n">
+        <f aca="false">SUM(G16:H16)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="11"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="23" t="n">
+        <f aca="false">SUM(G17:H17)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="11"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33" t="n">
+        <f aca="false">SUM(G18:H18)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="11"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="28" t="n">
+        <v>12</v>
+      </c>
+      <c r="I19" s="29" t="n">
+        <f aca="false">SUM(G19:H19)</f>
+        <v>12</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="38" t="n">
-        <f aca="false">SUM(G5:G15)</f>
+      <c r="G20" s="41" t="n">
+        <f aca="false">SUM(G5:G19)</f>
         <v>85</v>
       </c>
-      <c r="H16" s="38" t="n">
-        <f aca="false">SUM(H5:H15)</f>
+      <c r="H20" s="33" t="n">
+        <f aca="false">SUM(H5:H19)</f>
         <v>683</v>
       </c>
-      <c r="I16" s="39" t="n">
-        <f aca="false">SUM(G16:H16)</f>
+      <c r="I20" s="42" t="n">
+        <f aca="false">SUM(G20:H20)</f>
         <v>768</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
     <mergeCell ref="G2:H3"/>
-    <mergeCell ref="B5:B15"/>
+    <mergeCell ref="B5:B19"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="D5:D9"/>
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="C10:C14"/>
     <mergeCell ref="D10:D14"/>
     <mergeCell ref="E10:E13"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="E15:E18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
changed "too few" to "too few reads"
</commit_message>
<xml_diff>
--- a/SVGs/Table_2.xlsx
+++ b/SVGs/Table_2.xlsx
@@ -58,7 +58,8 @@
     <t xml:space="preserve">35-40</t>
   </si>
   <si>
-    <t xml:space="preserve">too few</t>
+    <t xml:space="preserve">too few
+reads</t>
   </si>
 </sst>
 </file>
@@ -494,7 +495,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -609,7 +610,7 @@
   <dimension ref="B1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -960,6 +961,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
+      <c r="Q16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="11"/>

</xml_diff>